<commit_message>
Add some information and complete the document.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Data to be processed (path)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results</t>
+    <t>Path of the pillar array info</t>
+  </si>
+  <si>
+    <t>Saving path</t>
+  </si>
+  <si>
+    <t>Exp date</t>
+  </si>
+  <si>
+    <t>Channel height (um)</t>
+  </si>
+  <si>
+    <t>Channel width (um)</t>
+  </si>
+  <si>
+    <t>Flow rate (nL/s)</t>
+  </si>
+  <si>
+    <t>Initial velocity (m/s)</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Figures</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Figures</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\circlesforPAs1_S10.mat</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\circlesforPAs2_S10.mat</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Shapes_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Shapes_2</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Shapes_1</t>
+  </si>
+  <si>
+    <t>Calibration (um/pixel)</t>
   </si>
 </sst>
 </file>
@@ -76,9 +115,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,31 +399,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44299</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>48</v>
+      </c>
+      <c r="F2">
+        <v>400</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <f>G2/F2/E2</f>
+        <v>2.6041666666666668E-5</v>
+      </c>
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>55</v>
+      </c>
+      <c r="F3">
+        <v>400</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">G3/F3/E3</f>
+        <v>2.2727272727272729E-5</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>400</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I4">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add experimental date on 2021-10-29
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -62,27 +62,9 @@
     <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\circlesforPAs2_S10.mat</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Shapes_1</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Shapes_2</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Shapes_1</t>
-  </si>
-  <si>
     <t>Calibration (um/pixel)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Shapes_1</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Shapes_1</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Shapes_2</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Figures</t>
   </si>
   <si>
@@ -99,6 +81,51 @@
   </si>
   <si>
     <t>Exposure time (ms)</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\circlesforPAs20211029_S15.mat</t>
+  </si>
+  <si>
+    <t>29/10/2021</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_3</t>
+  </si>
+  <si>
+    <t>13/04/2021</t>
+  </si>
+  <si>
+    <t>30/04/2021</t>
+  </si>
+  <si>
+    <t>25/09/2020</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Figures</t>
   </si>
 </sst>
 </file>
@@ -426,17 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -472,18 +499,18 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>44299</v>
+      <c r="A2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -512,11 +539,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44316</v>
+      <c r="A3" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -534,7 +561,7 @@
         <v>0.5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="0">G3/F3/E3</f>
+        <f t="shared" ref="H3:H10" si="0">G3/F3/E3</f>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I3">
@@ -545,11 +572,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>44316</v>
+      <c r="A4" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -578,17 +605,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>44099</v>
+      <c r="A5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -611,17 +638,17 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>44099</v>
+      <c r="A6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -645,16 +672,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>44105</v>
+        <v>43840</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -673,6 +700,105 @@
         <v>0.1</v>
       </c>
       <c r="J7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <v>400</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2.2727272727272729E-5</v>
+      </c>
+      <c r="I8">
+        <v>0.1</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>400</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>55</v>
+      </c>
+      <c r="F10">
+        <v>400</v>
+      </c>
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>6.8181818181818184E-5</v>
+      </c>
+      <c r="I10">
+        <v>0.1</v>
+      </c>
+      <c r="J10">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add experimental data on 2021-10-29
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -62,27 +62,9 @@
     <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\circlesforPAs2_S10.mat</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Shapes_1</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Shapes_2</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Shapes_1</t>
-  </si>
-  <si>
     <t>Calibration (um/pixel)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Shapes_1</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Shapes_1</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Shapes_2</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Figures</t>
   </si>
   <si>
@@ -99,6 +81,51 @@
   </si>
   <si>
     <t>Exposure time (ms)</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\circlesforPAs20211029_S15.mat</t>
+  </si>
+  <si>
+    <t>29/10/2021</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_3</t>
+  </si>
+  <si>
+    <t>13/04/2021</t>
+  </si>
+  <si>
+    <t>30/04/2021</t>
+  </si>
+  <si>
+    <t>25/09/2020</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Figures</t>
   </si>
 </sst>
 </file>
@@ -426,17 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -472,18 +499,18 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>44299</v>
+      <c r="A2" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -512,11 +539,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44316</v>
+      <c r="A3" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -534,7 +561,7 @@
         <v>0.5</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="0">G3/F3/E3</f>
+        <f t="shared" ref="H3:H10" si="0">G3/F3/E3</f>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I3">
@@ -545,11 +572,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>44316</v>
+      <c r="A4" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -578,17 +605,17 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>44099</v>
+      <c r="A5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -611,17 +638,17 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>44099</v>
+      <c r="A6" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -645,16 +672,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>44105</v>
+        <v>43840</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -673,6 +700,105 @@
         <v>0.1</v>
       </c>
       <c r="J7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <v>400</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2.2727272727272729E-5</v>
+      </c>
+      <c r="I8">
+        <v>0.1</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <v>55</v>
+      </c>
+      <c r="F9">
+        <v>400</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>55</v>
+      </c>
+      <c r="F10">
+        <v>400</v>
+      </c>
+      <c r="G10">
+        <v>1.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>6.8181818181818184E-5</v>
+      </c>
+      <c r="I10">
+        <v>0.1</v>
+      </c>
+      <c r="J10">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Sheet2 for the Dynamics_viscoelasticity.m code.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -50,12 +51,6 @@
     <t>Initial velocity (m/s)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Figures</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Figures</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\circlesforPAs1_S10.mat</t>
   </si>
   <si>
@@ -65,12 +60,6 @@
     <t>Calibration (um/pixel)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Figures</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Figures</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\circlesforPAs1.mat</t>
   </si>
   <si>
@@ -125,7 +114,28 @@
     <t>25/09/2020</t>
   </si>
   <si>
-    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Figures</t>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Classification manually 20210413-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Classification manually 20210430-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Classification manually 20211029-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20210413-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20210430-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20200925-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20201001-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20211029-Actin\Figures</t>
   </si>
 </sst>
 </file>
@@ -455,16 +465,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
@@ -499,24 +509,24 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>48</v>
@@ -540,16 +550,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>55</v>
@@ -573,16 +583,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>55</v>
@@ -606,16 +616,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -639,16 +649,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -675,13 +685,13 @@
         <v>43840</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -705,16 +715,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>55</v>
@@ -738,16 +748,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>55</v>
@@ -771,16 +781,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>55</v>
@@ -806,4 +816,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Classification of dynamic modes and buckling types.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -50,12 +51,6 @@
     <t>Initial velocity (m/s)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Figures</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Figures</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\circlesforPAs1_S10.mat</t>
   </si>
   <si>
@@ -65,12 +60,6 @@
     <t>Calibration (um/pixel)</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Figures</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Figures</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\circlesforPAs1.mat</t>
   </si>
   <si>
@@ -125,7 +114,28 @@
     <t>25/09/2020</t>
   </si>
   <si>
-    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Figures</t>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Classification manually 20210413-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Classification manually 20210430-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Classification manually 20211029-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20210413-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20210430-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20200925-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20201001-Actin\Figures</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20211029-Actin\Figures</t>
   </si>
 </sst>
 </file>
@@ -455,16 +465,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
@@ -499,24 +509,24 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>48</v>
@@ -540,16 +550,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E3">
         <v>55</v>
@@ -573,16 +583,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>55</v>
@@ -606,16 +616,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -639,16 +649,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -675,13 +685,13 @@
         <v>43840</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>30</v>
@@ -705,16 +715,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>55</v>
@@ -738,16 +748,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>55</v>
@@ -771,16 +781,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>55</v>
@@ -806,4 +816,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add 20200925 & 20201001 in sheet2.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin - Copy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\GitHub\Postprocessing_Actin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>E:\Dropbox\Research\All Plottings\20211029-Actin\Figures</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Classification manually 20201001-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Classification manually 20200925-Actin.xlsx</t>
   </si>
 </sst>
 </file>
@@ -466,7 +472,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,10 +826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,6 +889,22 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add 20220104 data and sort the lists.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -111,9 +111,6 @@
     <t>30/04/2021</t>
   </si>
   <si>
-    <t>25/09/2020</t>
-  </si>
-  <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Classification manually 20210413-Actin.xlsx</t>
   </si>
   <si>
@@ -142,12 +139,24 @@
   </si>
   <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Classification manually 20200925-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20220104-Actin\Figures</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\circlesforPAs20220104_S15.mat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,10 +194,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,96 +532,96 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
+      <c r="A2" s="3">
+        <v>44099</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>400</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f>G2/F2/E2</f>
-        <v>2.6041666666666668E-5</v>
+        <v>8.3333333333333331E-5</v>
       </c>
       <c r="I2">
         <v>0.1</v>
       </c>
       <c r="J2">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
+      <c r="A3" s="3">
+        <v>44099</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
       <c r="E3">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>400</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="0">G3/F3/E3</f>
-        <v>2.2727272727272729E-5</v>
+        <f>G3/F3/E3</f>
+        <v>8.3333333333333331E-5</v>
       </c>
       <c r="I3">
         <v>0.1</v>
       </c>
       <c r="J3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44105</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F4">
         <v>400</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
-        <v>4.5454545454545459E-5</v>
+        <f>G4/F4/E4</f>
+        <v>4.1666666666666665E-5</v>
       </c>
       <c r="I4">
         <v>0.1</v>
@@ -621,96 +631,96 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
+      <c r="A5" s="3">
+        <v>44299</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F5">
         <v>400</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333331E-5</v>
+        <f>G5/F5/E5</f>
+        <v>2.6041666666666668E-5</v>
       </c>
       <c r="I5">
         <v>0.1</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
+      <c r="A6" s="3">
+        <v>44316</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>400</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333331E-5</v>
+        <f>G6/F6/E6</f>
+        <v>2.2727272727272729E-5</v>
       </c>
       <c r="I6">
         <v>0.1</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>43840</v>
+      <c r="A7" s="3">
+        <v>44316</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F7">
         <v>400</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>4.1666666666666665E-5</v>
+        <f>G7/F7/E7</f>
+        <v>4.5454545454545459E-5</v>
       </c>
       <c r="I7">
         <v>0.1</v>
@@ -720,8 +730,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
+      <c r="A8" s="3">
+        <v>44498</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -730,7 +740,7 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>55</v>
@@ -742,7 +752,7 @@
         <v>0.5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>G8/F8/E8</f>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I8">
@@ -753,8 +763,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
+      <c r="A9" s="3">
+        <v>44498</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
@@ -763,7 +773,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <v>55</v>
@@ -775,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f>G9/F9/E9</f>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I9">
@@ -786,8 +796,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
+      <c r="A10" s="3">
+        <v>44498</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -796,7 +806,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>55</v>
@@ -808,7 +818,7 @@
         <v>1.5</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f>G10/F10/E10</f>
         <v>6.8181818181818184E-5</v>
       </c>
       <c r="I10">
@@ -818,7 +828,220 @@
         <v>20</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>55</v>
+      </c>
+      <c r="F11">
+        <v>400</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f>G11/F11/E11</f>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I11">
+        <v>0.1</v>
+      </c>
+      <c r="J11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
   </sheetData>
+  <sortState ref="A2:J10">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -828,7 +1051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -857,55 +1080,58 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:C6">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add 20220104 in sheet2.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\circlesforPAs20220104_S15.mat</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\Classification manually 20220104-Actin.xlsx</t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -198,7 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -554,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <f>G2/F2/E2</f>
+        <f t="shared" ref="H2:H11" si="0">G2/F2/E2</f>
         <v>8.3333333333333331E-5</v>
       </c>
       <c r="I2">
@@ -587,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <f>G3/F3/E3</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333331E-5</v>
       </c>
       <c r="I3">
@@ -620,7 +623,7 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f>G4/F4/E4</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666665E-5</v>
       </c>
       <c r="I4">
@@ -653,7 +656,7 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f>G5/F5/E5</f>
+        <f t="shared" si="0"/>
         <v>2.6041666666666668E-5</v>
       </c>
       <c r="I5">
@@ -686,7 +689,7 @@
         <v>0.5</v>
       </c>
       <c r="H6">
-        <f>G6/F6/E6</f>
+        <f t="shared" si="0"/>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I6">
@@ -719,7 +722,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <f>G7/F7/E7</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I7">
@@ -752,7 +755,7 @@
         <v>0.5</v>
       </c>
       <c r="H8">
-        <f>G8/F8/E8</f>
+        <f t="shared" si="0"/>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I8">
@@ -785,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <f>G9/F9/E9</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I9">
@@ -818,7 +821,7 @@
         <v>1.5</v>
       </c>
       <c r="H10">
-        <f>G10/F10/E10</f>
+        <f t="shared" si="0"/>
         <v>6.8181818181818184E-5</v>
       </c>
       <c r="I10">
@@ -851,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <f>G11/F11/E11</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I11">
@@ -1049,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,6 +1131,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C6">
     <sortCondition ref="B1"/>

</xml_diff>

<commit_message>
add ExpDate in sheet2.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -93,9 +93,6 @@
     <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\circlesforPAs20211029_S15.mat</t>
   </si>
   <si>
-    <t>29/10/2021</t>
-  </si>
-  <si>
     <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_1</t>
   </si>
   <si>
@@ -103,12 +100,6 @@
   </si>
   <si>
     <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_3</t>
-  </si>
-  <si>
-    <t>13/04/2021</t>
-  </si>
-  <si>
-    <t>30/04/2021</t>
   </si>
   <si>
     <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Classification manually 20210413-Actin.xlsx</t>
@@ -197,10 +188,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -485,7 +475,7 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +525,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>44099</v>
       </c>
       <c r="B2" t="s">
@@ -545,7 +535,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -568,7 +558,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>44099</v>
       </c>
       <c r="B3" t="s">
@@ -578,7 +568,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -601,7 +591,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>44105</v>
       </c>
       <c r="B4" t="s">
@@ -611,7 +601,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -634,7 +624,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>44299</v>
       </c>
       <c r="B5" t="s">
@@ -644,7 +634,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>48</v>
@@ -667,7 +657,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>44316</v>
       </c>
       <c r="B6" t="s">
@@ -677,7 +667,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E6">
         <v>55</v>
@@ -700,7 +690,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>44316</v>
       </c>
       <c r="B7" t="s">
@@ -710,7 +700,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>55</v>
@@ -733,17 +723,17 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>44498</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <v>55</v>
@@ -766,17 +756,17 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>44498</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9">
         <v>55</v>
@@ -799,17 +789,17 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>44498</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <v>55</v>
@@ -832,17 +822,17 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>44565</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <v>55</v>
@@ -865,181 +855,181 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="2"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="2"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="2"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="2"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="2"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="2"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="2"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="2"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="2"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="2"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="2"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="2"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
+      <c r="A48" s="2"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="2"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+      <c r="A50" s="2"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="A51" s="2"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
+      <c r="A52" s="2"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="2"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="2"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="2"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
+      <c r="A58" s="2"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
+      <c r="A59" s="2"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
+      <c r="A60" s="2"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
+      <c r="A61" s="2"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
+      <c r="A62" s="2"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
+      <c r="A63" s="2"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
+      <c r="A64" s="2"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
+      <c r="A65" s="2"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
+      <c r="A66" s="2"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
+      <c r="A67" s="2"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
+      <c r="A68" s="2"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
+      <c r="A69" s="2"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
+      <c r="A70" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:J10">
@@ -1052,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,61 +1073,253 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44099</v>
+      </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44105</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44299</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44498</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44565</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:C6">

</xml_diff>

<commit_message>
Add pillar array types in sheet1 & sheet2.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\Classification manually 20220104-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>Pillar array types</t>
+  </si>
+  <si>
+    <t>OldMask_Square_Phi20_Gap10_FlowAng0</t>
+  </si>
+  <si>
+    <t>OldMask_Square_Phi20_Gap5_FlowAng0</t>
+  </si>
+  <si>
+    <t>CrMask_Rhombic_Phi20_Gap10_FlowAng0</t>
+  </si>
+  <si>
+    <t>CrMask_Rhombic_Phi20_Gap15_FlowAng0</t>
   </si>
 </sst>
 </file>
@@ -472,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,9 +505,10 @@
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -523,8 +539,11 @@
       <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44099</v>
       </c>
@@ -556,8 +575,11 @@
       <c r="J2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44099</v>
       </c>
@@ -589,8 +611,11 @@
       <c r="J3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44105</v>
       </c>
@@ -622,8 +647,11 @@
       <c r="J4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44299</v>
       </c>
@@ -655,8 +683,11 @@
       <c r="J5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44316</v>
       </c>
@@ -688,8 +719,11 @@
       <c r="J6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44316</v>
       </c>
@@ -721,8 +755,11 @@
       <c r="J7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44498</v>
       </c>
@@ -754,8 +791,11 @@
       <c r="J8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44498</v>
       </c>
@@ -787,8 +827,11 @@
       <c r="J9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44498</v>
       </c>
@@ -820,8 +863,11 @@
       <c r="J10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44565</v>
       </c>
@@ -853,20 +899,23 @@
       <c r="J11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1042,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1102,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
@@ -1061,7 +1110,7 @@
     <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1071,8 +1120,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44099</v>
       </c>
@@ -1082,8 +1134,11 @@
       <c r="C2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44105</v>
       </c>
@@ -1093,8 +1148,11 @@
       <c r="C3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44299</v>
       </c>
@@ -1104,8 +1162,11 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44316</v>
       </c>
@@ -1115,8 +1176,11 @@
       <c r="C5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44498</v>
       </c>
@@ -1126,8 +1190,11 @@
       <c r="C6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44565</v>
       </c>
@@ -1137,26 +1204,29 @@
       <c r="C7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add pillar array type labels in sheet2.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>CrMask_Rhombic_Phi20_Gap15_FlowAng0</t>
+  </si>
+  <si>
+    <t>Pillar array type labels</t>
   </si>
 </sst>
 </file>
@@ -489,7 +492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
@@ -1091,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1113,7 @@
     <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1123,8 +1126,11 @@
       <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44099</v>
       </c>
@@ -1137,8 +1143,11 @@
       <c r="D2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44105</v>
       </c>
@@ -1151,8 +1160,11 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44299</v>
       </c>
@@ -1165,8 +1177,11 @@
       <c r="D4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44316</v>
       </c>
@@ -1179,8 +1194,11 @@
       <c r="D5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44498</v>
       </c>
@@ -1193,8 +1211,11 @@
       <c r="D6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44565</v>
       </c>
@@ -1207,26 +1228,29 @@
       <c r="D7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add more information about the pillar array.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Pillar array type labels</t>
+  </si>
+  <si>
+    <t>Center-to-center distance</t>
+  </si>
+  <si>
+    <t>Pillar diameter</t>
   </si>
 </sst>
 </file>
@@ -490,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,9 +515,11 @@
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -545,8 +553,14 @@
       <c r="K1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44099</v>
       </c>
@@ -581,8 +595,14 @@
       <c r="K2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>30</v>
+      </c>
+      <c r="M2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44099</v>
       </c>
@@ -617,8 +637,14 @@
       <c r="K3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>30</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44105</v>
       </c>
@@ -653,8 +679,14 @@
       <c r="K4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>25</v>
+      </c>
+      <c r="M4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44299</v>
       </c>
@@ -689,8 +721,14 @@
       <c r="K5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>30</v>
+      </c>
+      <c r="M5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44316</v>
       </c>
@@ -725,8 +763,14 @@
       <c r="K6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>30</v>
+      </c>
+      <c r="M6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44316</v>
       </c>
@@ -761,8 +805,14 @@
       <c r="K7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44498</v>
       </c>
@@ -797,8 +847,14 @@
       <c r="K8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>35</v>
+      </c>
+      <c r="M8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44498</v>
       </c>
@@ -833,8 +889,14 @@
       <c r="K9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>35</v>
+      </c>
+      <c r="M9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44498</v>
       </c>
@@ -869,8 +931,14 @@
       <c r="K10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>35</v>
+      </c>
+      <c r="M10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44565</v>
       </c>
@@ -905,20 +973,26 @@
       <c r="K11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>35</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1096,7 +1170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add 20210914 data. Change the paths in the second column in sheet2.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -102,15 +102,6 @@
     <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Group_3</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210413-Actin\results\Classification manually 20210413-Actin.xlsx</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20210430-Actin\results\Classification manually 20210430-Actin.xlsx</t>
-  </si>
-  <si>
-    <t>G:\PhD, PMMH, ESPCI\Processing\20211029-Actin\results\Classification manually 20211029-Actin.xlsx</t>
-  </si>
-  <si>
     <t>E:\Dropbox\Research\All Plottings\20210413-Actin\Figures</t>
   </si>
   <si>
@@ -126,12 +117,6 @@
     <t>E:\Dropbox\Research\All Plottings\20211029-Actin\Figures</t>
   </si>
   <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20201001-Actin\results\Classification manually 20201001-Actin.xlsx</t>
-  </si>
-  <si>
-    <t>F:\PhD, PMMH, ESPCI\Processing\20200925-Actin\results\Classification manually 20200925-Actin.xlsx</t>
-  </si>
-  <si>
     <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\Group_1</t>
   </si>
   <si>
@@ -141,9 +126,6 @@
     <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\circlesforPAs20220104_S15.mat</t>
   </si>
   <si>
-    <t>G:\PhD, PMMH, ESPCI\Processing\20220104-Actin\results\Classification manually 20220104-Actin.xlsx</t>
-  </si>
-  <si>
     <t>Pillar array types</t>
   </si>
   <si>
@@ -166,6 +148,42 @@
   </si>
   <si>
     <t>Pillar diameter</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20210914-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20210914-Actin\results\circlesforPAs20210914_G10.mat</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20210914-Actin\Figures</t>
+  </si>
+  <si>
+    <t>CrMask_Square_Phi20_Gap10_FlowAng0</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20210914-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20200925-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20201001-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20210413-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20210430-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20211029-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20220104-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20210914-Actin.xlsx</t>
   </si>
 </sst>
 </file>
@@ -212,10 +230,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,13 +570,13 @@
         <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -571,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -583,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H11" si="0">G2/F2/E2</f>
+        <f>G2/F2/E2</f>
         <v>8.3333333333333331E-5</v>
       </c>
       <c r="I2">
@@ -593,7 +612,7 @@
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L2">
         <v>30</v>
@@ -613,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -625,7 +644,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f>G3/F3/E3</f>
         <v>8.3333333333333331E-5</v>
       </c>
       <c r="I3">
@@ -635,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L3">
         <v>30</v>
@@ -655,7 +674,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -667,7 +686,7 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f>G4/F4/E4</f>
         <v>4.1666666666666665E-5</v>
       </c>
       <c r="I4">
@@ -677,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L4">
         <v>25</v>
@@ -697,7 +716,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <v>48</v>
@@ -709,7 +728,7 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f>G5/F5/E5</f>
         <v>2.6041666666666668E-5</v>
       </c>
       <c r="I5">
@@ -719,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L5">
         <v>30</v>
@@ -739,7 +758,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>55</v>
@@ -751,7 +770,7 @@
         <v>0.5</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>G6/F6/E6</f>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I6">
@@ -761,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L6">
         <v>30</v>
@@ -781,7 +800,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7">
         <v>55</v>
@@ -793,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>G7/F7/E7</f>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I7">
@@ -803,7 +822,7 @@
         <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="L7">
         <v>30</v>
@@ -814,16 +833,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>44498</v>
+        <v>44453</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E8">
         <v>55</v>
@@ -834,9 +853,8 @@
       <c r="G8">
         <v>0.5</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>2.2727272727272729E-5</v>
+      <c r="H8" s="3">
+        <v>2.2727299999999998E-5</v>
       </c>
       <c r="I8">
         <v>0.1</v>
@@ -845,10 +863,10 @@
         <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L8">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M8">
         <v>20</v>
@@ -856,16 +874,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>44498</v>
+        <v>44453</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E9">
         <v>55</v>
@@ -876,9 +894,8 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>4.5454545454545459E-5</v>
+      <c r="H9" s="3">
+        <v>4.5454500000000003E-5</v>
       </c>
       <c r="I9">
         <v>0.1</v>
@@ -887,10 +904,10 @@
         <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="M9">
         <v>20</v>
@@ -901,13 +918,13 @@
         <v>44498</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10">
         <v>55</v>
@@ -916,11 +933,11 @@
         <v>400</v>
       </c>
       <c r="G10">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>6.8181818181818184E-5</v>
+        <f>G10/F10/E10</f>
+        <v>2.2727272727272729E-5</v>
       </c>
       <c r="I10">
         <v>0.1</v>
@@ -929,7 +946,7 @@
         <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L10">
         <v>35</v>
@@ -940,16 +957,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>44565</v>
+        <v>44498</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E11">
         <v>55</v>
@@ -961,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f>G11/F11/E11</f>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I11">
@@ -971,7 +988,7 @@
         <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L11">
         <v>35</v>
@@ -981,10 +998,88 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2">
+        <v>44498</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12">
+        <v>55</v>
+      </c>
+      <c r="F12">
+        <v>400</v>
+      </c>
+      <c r="G12">
+        <v>1.5</v>
+      </c>
+      <c r="H12">
+        <f>G12/F12/E12</f>
+        <v>6.8181818181818184E-5</v>
+      </c>
+      <c r="I12">
+        <v>0.1</v>
+      </c>
+      <c r="J12">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12">
+        <v>35</v>
+      </c>
+      <c r="M12">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>44565</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>55</v>
+      </c>
+      <c r="F13">
+        <v>400</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <f>G13/F13/E13</f>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I13">
+        <v>0.1</v>
+      </c>
+      <c r="J13">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13">
+        <v>35</v>
+      </c>
+      <c r="M13">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1158,7 +1253,7 @@
       <c r="A70" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:J10">
+  <sortState ref="A2:M70">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1170,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,10 +1293,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1209,13 +1304,13 @@
         <v>44099</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1226,13 +1321,13 @@
         <v>44105</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1243,13 +1338,13 @@
         <v>44299</v>
       </c>
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -1260,13 +1355,13 @@
         <v>44316</v>
       </c>
       <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1274,40 +1369,54 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>44498</v>
+        <v>44453</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>44565</v>
+        <v>44498</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>44565</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -1490,8 +1599,8 @@
       <c r="A70" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:C6">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:E70">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add 20220216 & 20220217 data and flow angle column in Sheet1.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -184,6 +184,39 @@
   </si>
   <si>
     <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20210914-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220216-Actin\results\Group_3</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220216-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220216-Actin\results\Group_2</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20220216-Actin\Figures</t>
+  </si>
+  <si>
+    <t>CrMask_Square_Phi20_Gap10_FlowAng10</t>
+  </si>
+  <si>
+    <t>Flow angle</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220216-Actin\results\circlesforPAs20220216_T10.mat</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20220216-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\Manually classification documents\Classification manually 20220217-Actin.xlsx</t>
+  </si>
+  <si>
+    <t>E:\Dropbox\Research\All Plottings\20220217-Actin\Figures</t>
+  </si>
+  <si>
+    <t>CrMask_Square_Phi20_Gap10_FlowAng20</t>
   </si>
 </sst>
 </file>
@@ -515,17 +548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -536,9 +570,10 @@
     <col min="11" max="11" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -578,8 +613,11 @@
       <c r="M1" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44099</v>
       </c>
@@ -602,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <f>G2/F2/E2</f>
+        <f t="shared" ref="H2:H7" si="0">G2/F2/E2</f>
         <v>8.3333333333333331E-5</v>
       </c>
       <c r="I2">
@@ -620,8 +658,11 @@
       <c r="M2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44099</v>
       </c>
@@ -644,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <f>G3/F3/E3</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333331E-5</v>
       </c>
       <c r="I3">
@@ -662,8 +703,11 @@
       <c r="M3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44105</v>
       </c>
@@ -686,7 +730,7 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <f>G4/F4/E4</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666665E-5</v>
       </c>
       <c r="I4">
@@ -704,8 +748,11 @@
       <c r="M4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44299</v>
       </c>
@@ -728,7 +775,7 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <f>G5/F5/E5</f>
+        <f t="shared" si="0"/>
         <v>2.6041666666666668E-5</v>
       </c>
       <c r="I5">
@@ -746,8 +793,11 @@
       <c r="M5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44316</v>
       </c>
@@ -770,7 +820,7 @@
         <v>0.5</v>
       </c>
       <c r="H6">
-        <f>G6/F6/E6</f>
+        <f t="shared" si="0"/>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I6">
@@ -788,8 +838,11 @@
       <c r="M6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44316</v>
       </c>
@@ -812,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <f>G7/F7/E7</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545459E-5</v>
       </c>
       <c r="I7">
@@ -830,8 +883,11 @@
       <c r="M7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44453</v>
       </c>
@@ -871,8 +927,11 @@
       <c r="M8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44453</v>
       </c>
@@ -912,8 +971,11 @@
       <c r="M9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44498</v>
       </c>
@@ -954,8 +1016,11 @@
       <c r="M10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44498</v>
       </c>
@@ -996,8 +1061,11 @@
       <c r="M11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44498</v>
       </c>
@@ -1038,8 +1106,11 @@
       <c r="M12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44565</v>
       </c>
@@ -1080,15 +1151,144 @@
       <c r="M13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44608</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14">
+        <v>55</v>
+      </c>
+      <c r="F14">
+        <v>400</v>
+      </c>
+      <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
+        <f>G14/F14/E14</f>
+        <v>2.2727272727272729E-5</v>
+      </c>
+      <c r="I14">
+        <v>0.1</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14">
+        <v>30</v>
+      </c>
+      <c r="M14">
+        <v>20</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>44608</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15">
+        <v>55</v>
+      </c>
+      <c r="F15">
+        <v>400</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f>G15/F15/E15</f>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I15">
+        <v>0.1</v>
+      </c>
+      <c r="J15">
+        <v>20</v>
+      </c>
+      <c r="K15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L15">
+        <v>30</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>44608</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16">
+        <v>55</v>
+      </c>
+      <c r="F16">
+        <v>400</v>
+      </c>
+      <c r="G16">
+        <v>1.5</v>
+      </c>
+      <c r="H16">
+        <f>G16/F16/E16</f>
+        <v>6.8181818181818184E-5</v>
+      </c>
+      <c r="I16">
+        <v>0.1</v>
+      </c>
+      <c r="J16">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16">
+        <v>30</v>
+      </c>
+      <c r="M16">
+        <v>20</v>
+      </c>
+      <c r="N16">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -1266,13 +1466,14 @@
   <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.7109375" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1419,7 +1620,38 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2">
+        <v>44608</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44609</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>

<commit_message>
Add 20220217 0.5nL data.
</commit_message>
<xml_diff>
--- a/ForActinPostprocessing.xlsx
+++ b/ForActinPostprocessing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>Data to be processed (path)</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>G:\PhD, PMMH, ESPCI\Processing\20220217-Actin\results\circlesforPAs_T20_23.08.21_lowerone_30.mat</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220217-Actin\results\Group_1</t>
+  </si>
+  <si>
+    <t>G:\PhD, PMMH, ESPCI\Processing\20220217-Actin\results\circlesforPAs_T20_23.08.21_lowerone_2.mat</t>
   </si>
 </sst>
 </file>
@@ -557,11 +563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1013,7 @@
         <v>0.5</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H16" si="1">G10/F10/E10</f>
+        <f t="shared" ref="H10:H17" si="1">G10/F10/E10</f>
         <v>2.2727272727272729E-5</v>
       </c>
       <c r="I10">
@@ -1304,10 +1310,10 @@
         <v>44609</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
         <v>62</v>
@@ -1319,11 +1325,11 @@
         <v>400</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H17">
-        <f t="shared" ref="H17:H18" si="2">G17/F17/E17</f>
-        <v>4.5454545454545459E-5</v>
+        <f t="shared" si="1"/>
+        <v>2.2727272727272729E-5</v>
       </c>
       <c r="I17">
         <v>0.1</v>
@@ -1349,7 +1355,7 @@
         <v>44609</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
         <v>66</v>
@@ -1364,33 +1370,75 @@
         <v>400</v>
       </c>
       <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H19" si="2">G18/F18/E18</f>
+        <v>4.5454545454545459E-5</v>
+      </c>
+      <c r="I18">
+        <v>0.1</v>
+      </c>
+      <c r="J18">
+        <v>20</v>
+      </c>
+      <c r="K18" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18">
+        <v>30</v>
+      </c>
+      <c r="M18">
+        <v>20</v>
+      </c>
+      <c r="N18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44609</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19">
+        <v>55</v>
+      </c>
+      <c r="F19">
+        <v>400</v>
+      </c>
+      <c r="G19">
         <v>1.5</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <f t="shared" si="2"/>
         <v>6.8181818181818184E-5</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <v>0.1</v>
       </c>
-      <c r="J18">
-        <v>20</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="J19">
+        <v>20</v>
+      </c>
+      <c r="K19" t="s">
         <v>63</v>
       </c>
-      <c r="L18">
+      <c r="L19">
         <v>30</v>
       </c>
-      <c r="M18">
-        <v>20</v>
-      </c>
-      <c r="N18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="M19">
+        <v>20</v>
+      </c>
+      <c r="N19">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1544,6 +1592,9 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:M70">
@@ -1558,9 +1609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>